<commit_message>
add pid position function
</commit_message>
<xml_diff>
--- a/Bill.xlsx
+++ b/Bill.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1. Phenikaa University\AML\0. Project\5. MicroMouse\3. Github Repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B68FEF-5E9E-4D4B-B3C0-2495AC00D5F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A84BF2DD-9C31-43C3-B04B-F828A0D0D747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D07DEA89-26FB-4652-A59A-55D5EE707AA7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>STT</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>Trục 5mm</t>
+  </si>
+  <si>
+    <t>Bánh bi</t>
   </si>
 </sst>
 </file>
@@ -462,7 +465,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -513,7 +516,7 @@
       </c>
       <c r="G2" s="3">
         <f>SUM(E:E)</f>
-        <v>850750</v>
+        <v>906250</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -661,9 +664,21 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
+        <v>55500</v>
+      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>55500</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix laser sensor issue
</commit_message>
<xml_diff>
--- a/Bill.xlsx
+++ b/Bill.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1. Phenikaa University\AML\0. Project\5. MicroMouse\3. Github Repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A84BF2DD-9C31-43C3-B04B-F828A0D0D747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A949054-F5C2-4DAA-9B8C-BD05D83B436E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D07DEA89-26FB-4652-A59A-55D5EE707AA7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>STT</t>
   </si>
@@ -80,7 +80,10 @@
     <t>Trục 5mm</t>
   </si>
   <si>
-    <t>Bánh bi</t>
+    <t>Bi mắt trâu</t>
+  </si>
+  <si>
+    <t>Thành tiền</t>
   </si>
 </sst>
 </file>
@@ -115,15 +118,21 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -131,11 +140,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -144,6 +168,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -465,7 +495,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -480,7 +510,7 @@
     <col min="8" max="9" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -494,10 +524,10 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -514,12 +544,9 @@
         <f>C2*D2</f>
         <v>60000</v>
       </c>
-      <c r="G2" s="3">
-        <f>SUM(E:E)</f>
-        <v>906250</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -537,7 +564,7 @@
         <v>156700</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -555,7 +582,7 @@
         <v>139050</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -573,7 +600,7 @@
         <v>118000</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -590,8 +617,11 @@
         <f t="shared" si="0"/>
         <v>59000</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I6" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -608,8 +638,12 @@
         <f t="shared" si="0"/>
         <v>144000</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I7" s="5">
+        <f>SUM(E:E)</f>
+        <v>890750</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -627,7 +661,7 @@
         <v>84000</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -645,7 +679,7 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -663,7 +697,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -671,29 +705,29 @@
         <v>14</v>
       </c>
       <c r="C11" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" s="1">
-        <v>55500</v>
+        <v>20000</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>55500</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E12" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E13" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E14" s="1">
         <f t="shared" si="0"/>
         <v>0</v>

</xml_diff>

<commit_message>
added some function && completed Run() in main.c
</commit_message>
<xml_diff>
--- a/Bill.xlsx
+++ b/Bill.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1. Phenikaa University\AML\0. Project\5. MicroMouse\3. Github Repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D45480-0629-4B42-BF98-3CCBD51D4518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83E47A8-6A07-41B8-97A7-41525D2ED3DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D07DEA89-26FB-4652-A59A-55D5EE707AA7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>STT</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>Vòng bi 625</t>
+  </si>
+  <si>
+    <t>Người mua</t>
   </si>
 </sst>
 </file>
@@ -510,7 +513,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -541,6 +544,9 @@
       <c r="E1" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">

</xml_diff>